<commit_message>
This is a review for the log sheet to be modified to have a fixed format
</commit_message>
<xml_diff>
--- a/Documents/Review Log V 2.0.xlsx
+++ b/Documents/Review Log V 2.0.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="72">
   <si>
     <t>Review Log</t>
   </si>
@@ -191,6 +191,56 @@
   </si>
   <si>
     <t>( should be confirmed with customer  )</t>
+  </si>
+  <si>
+    <t>Review-16</t>
+  </si>
+  <si>
+    <t>Review-17</t>
+  </si>
+  <si>
+    <t>Review-18</t>
+  </si>
+  <si>
+    <t>Review-19</t>
+  </si>
+  <si>
+    <t>Review-20</t>
+  </si>
+  <si>
+    <t>Review-21</t>
+  </si>
+  <si>
+    <t>Review-22</t>
+  </si>
+  <si>
+    <t>Review-23</t>
+  </si>
+  <si>
+    <t>Review-24</t>
+  </si>
+  <si>
+    <t>18/04/2018</t>
+  </si>
+  <si>
+    <t>Ahmed Osama</t>
+  </si>
+  <si>
+    <t>Mahmoud Ibrahim</t>
+  </si>
+  <si>
+    <t>Need Modification</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The review log Needs some modifications :
+1- New Column must be added for Section Number 
+2- Doc ID must be Drop down menu with Certain IDs according to doc structure 
+3- Dates format must be fixed
+4- Source column must be Drop down menu according to doc structure 
+5- All names must be Drop down menu with Certain
+6- All Status column must be Drop down menu with fixed status with colors.
+7- Header row would be better if it's floating with you downwards
+</t>
   </si>
 </sst>
 </file>
@@ -317,21 +367,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -348,6 +389,18 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -653,10 +706,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J17"/>
+  <dimension ref="A1:J26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView tabSelected="1" topLeftCell="G13" workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -674,18 +727,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
-      <c r="J1" s="5"/>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
+      <c r="J1" s="10"/>
     </row>
     <row r="2" spans="1:10" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
@@ -720,390 +773,453 @@
       </c>
     </row>
     <row r="3" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="6">
+      <c r="B3" s="3">
         <v>1.2</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="D3" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="E3" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="F3" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="G3" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="H3" s="9" t="s">
+      <c r="D3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="H3" s="6" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="D4" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="E4" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="F4" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="G4" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="H4" s="6" t="s">
+      <c r="D4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="H4" s="3" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="D5" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="E5" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="F5" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="G5" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="H5" s="6" t="s">
+      <c r="D5" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="H5" s="3" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="10" t="s">
+      <c r="A6" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="B6" s="10" t="s">
+      <c r="B6" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="C6" s="10" t="s">
+      <c r="C6" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="D6" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="E6" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="F6" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="G6" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="H6" s="10" t="s">
+      <c r="D6" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="H6" s="7" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="10" t="s">
+      <c r="A7" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="B7" s="10" t="s">
+      <c r="B7" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="C7" s="10" t="s">
+      <c r="C7" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="D7" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="E7" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="F7" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="G7" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="H7" s="6" t="s">
+      <c r="D7" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="H7" s="3" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="10" t="s">
+      <c r="A8" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="B8" s="10" t="s">
+      <c r="B8" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="C8" s="10" t="s">
+      <c r="C8" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="D8" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="E8" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="F8" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="G8" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="H8" s="6" t="s">
+      <c r="D8" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="H8" s="3" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="10" t="s">
+      <c r="A9" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="B9" s="10" t="s">
+      <c r="B9" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="C9" s="10" t="s">
+      <c r="C9" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="D9" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="E9" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="F9" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="G9" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="H9" s="7" t="s">
+      <c r="D9" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="H9" s="4" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="10" t="s">
+      <c r="A10" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="B10" s="10" t="s">
+      <c r="B10" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="C10" s="10" t="s">
+      <c r="C10" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="D10" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="E10" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="F10" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="G10" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="H10" s="6" t="s">
+      <c r="D10" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F10" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="H10" s="3" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="10" t="s">
+      <c r="A11" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="B11" s="10" t="s">
+      <c r="B11" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="C11" s="10" t="s">
+      <c r="C11" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="D11" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="E11" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="F11" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="G11" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="H11" s="6" t="s">
+      <c r="D11" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F11" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="H11" s="3" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="10" t="s">
+      <c r="A12" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="B12" s="10" t="s">
+      <c r="B12" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="C12" s="10" t="s">
+      <c r="C12" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="D12" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="E12" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="F12" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="G12" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="H12" s="7" t="s">
+      <c r="D12" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E12" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F12" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="H12" s="4" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="10" t="s">
+      <c r="A13" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="B13" s="10" t="s">
+      <c r="B13" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="C13" s="10" t="s">
+      <c r="C13" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="D13" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="E13" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="F13" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="G13" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="H13" s="6" t="s">
+      <c r="D13" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F13" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="H13" s="3" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="10" t="s">
+      <c r="A14" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="B14" s="10" t="s">
+      <c r="B14" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="C14" s="10" t="s">
+      <c r="C14" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="D14" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="E14" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="F14" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="G14" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="H14" s="6" t="s">
+      <c r="D14" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E14" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F14" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="H14" s="3" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="10" t="s">
+      <c r="A15" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="B15" s="10" t="s">
+      <c r="B15" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="C15" s="10" t="s">
+      <c r="C15" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="D15" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="E15" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="F15" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="G15" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="H15" s="6" t="s">
+      <c r="D15" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E15" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F15" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="H15" s="3" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="10" t="s">
+      <c r="A16" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="B16" s="10" t="s">
+      <c r="B16" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="C16" s="8" t="s">
+      <c r="C16" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="D16" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="E16" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="F16" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="G16" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="H16" s="6" t="s">
+      <c r="D16" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E16" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F16" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="H16" s="3" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="10" t="s">
+      <c r="A17" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="B17" s="6">
+      <c r="B17" s="3">
         <v>2.5</v>
       </c>
-      <c r="D17" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="E17" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="F17" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="G17" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="H17" s="6" t="s">
+      <c r="D17" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E17" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F17" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="G17" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="H17" s="3" t="s">
         <v>57</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="195" x14ac:dyDescent="0.25">
+      <c r="A18" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="D18" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="E18" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="F18" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="G18" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="H18" s="11" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="7" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" s="7" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" s="7" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" s="7" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" s="7" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" s="7" t="s">
+        <v>66</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
This is a review on the Project repository to have unified structure and conventional naming system.
</commit_message>
<xml_diff>
--- a/Documents/Review Log V 2.0.xlsx
+++ b/Documents/Review Log V 2.0.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="74">
   <si>
     <t>Review Log</t>
   </si>
@@ -241,6 +241,12 @@
 6- All Status column must be Drop down menu with fixed status with colors.
 7- Header row would be better if it's floating with you downwards
 </t>
+  </si>
+  <si>
+    <t>Git Hub Project Structure</t>
+  </si>
+  <si>
+    <t>The Project repository  needs to be organized (documents must have unified  format DocName_ID without any Version number (this one will be a tag on the tool) )</t>
   </si>
 </sst>
 </file>
@@ -390,6 +396,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -397,9 +406,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -708,8 +714,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G13" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+    <sheetView tabSelected="1" topLeftCell="C13" workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -727,18 +733,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
-      <c r="H1" s="9"/>
-      <c r="I1" s="9"/>
-      <c r="J1" s="10"/>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+      <c r="H1" s="10"/>
+      <c r="I1" s="10"/>
+      <c r="J1" s="11"/>
     </row>
     <row r="2" spans="1:10" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
@@ -1178,13 +1184,31 @@
       <c r="G18" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="H18" s="11" t="s">
+      <c r="H18" s="8" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
         <v>59</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="D19" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="E19" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="F19" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="G19" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="H19" s="8" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>